<commit_message>
Added minor changes for demo
</commit_message>
<xml_diff>
--- a/static/upload/temp_timetable.xlsx
+++ b/static/upload/temp_timetable.xlsx
@@ -421,10 +421,10 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,7 +742,7 @@
     <row customHeight="1" ht="18" r="1" s="2">
       <c r="A1" s="43" t="inlineStr">
         <is>
-          <t>15/08/2019</t>
+          <t>16/09/2019</t>
         </is>
       </c>
       <c r="B1" s="31" t="inlineStr">
@@ -949,54 +949,18 @@
           <t>WP-II B316 teacher4 B4</t>
         </is>
       </c>
-      <c r="J13" s="48" t="inlineStr">
-        <is>
-          <t>WP-II B314 teacher4 B1</t>
-        </is>
-      </c>
-      <c r="K13" s="48" t="inlineStr">
-        <is>
-          <t>OS B317 teacher1 B2</t>
-        </is>
-      </c>
-      <c r="L13" s="48" t="inlineStr">
-        <is>
-          <t>OOSE B315 teacher2 B3</t>
-        </is>
-      </c>
-      <c r="M13" s="48" t="inlineStr">
-        <is>
-          <t>AD B313 admin B4</t>
-        </is>
-      </c>
-      <c r="N13" s="50" t="inlineStr">
-        <is>
-          <t>CG B305 teacher3</t>
-        </is>
-      </c>
-      <c r="O13" s="51" t="n"/>
-      <c r="P13" s="51" t="n"/>
-      <c r="Q13" s="51" t="n"/>
-      <c r="R13" s="48" t="inlineStr">
-        <is>
-          <t>CG B310 teacher3 B1</t>
-        </is>
-      </c>
-      <c r="S13" s="48" t="inlineStr">
-        <is>
-          <t>WP-II B313 teacher4 B2</t>
-        </is>
-      </c>
-      <c r="T13" s="52" t="inlineStr">
-        <is>
-          <t>OS B317 teacher1 B3</t>
-        </is>
-      </c>
-      <c r="U13" s="48" t="inlineStr">
-        <is>
-          <t>OOSE B315 teacher2 B4</t>
-        </is>
-      </c>
+      <c r="J13" s="12" t="n"/>
+      <c r="K13" s="15" t="n"/>
+      <c r="L13" s="15" t="n"/>
+      <c r="M13" s="16" t="n"/>
+      <c r="N13" s="12" t="n"/>
+      <c r="O13" s="15" t="n"/>
+      <c r="P13" s="15" t="n"/>
+      <c r="Q13" s="16" t="n"/>
+      <c r="R13" s="12" t="n"/>
+      <c r="S13" s="15" t="n"/>
+      <c r="T13" s="22" t="n"/>
+      <c r="U13" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="14" s="2">
       <c r="A14" s="42" t="inlineStr">
@@ -1005,30 +969,26 @@
 12:30</t>
         </is>
       </c>
-      <c r="B14" s="51" t="n"/>
-      <c r="C14" s="51" t="n"/>
-      <c r="D14" s="51" t="n"/>
-      <c r="E14" s="51" t="n"/>
-      <c r="F14" s="51" t="n"/>
-      <c r="G14" s="51" t="n"/>
-      <c r="H14" s="51" t="n"/>
-      <c r="I14" s="51" t="n"/>
-      <c r="J14" s="51" t="n"/>
-      <c r="K14" s="51" t="n"/>
-      <c r="L14" s="51" t="n"/>
-      <c r="M14" s="51" t="n"/>
-      <c r="N14" s="50" t="inlineStr">
-        <is>
-          <t>OOSE B305 teacher2</t>
-        </is>
-      </c>
-      <c r="O14" s="51" t="n"/>
-      <c r="P14" s="51" t="n"/>
-      <c r="Q14" s="51" t="n"/>
-      <c r="R14" s="51" t="n"/>
-      <c r="S14" s="51" t="n"/>
-      <c r="T14" s="51" t="n"/>
-      <c r="U14" s="51" t="n"/>
+      <c r="B14" s="50" t="n"/>
+      <c r="C14" s="50" t="n"/>
+      <c r="D14" s="50" t="n"/>
+      <c r="E14" s="50" t="n"/>
+      <c r="F14" s="50" t="n"/>
+      <c r="G14" s="50" t="n"/>
+      <c r="H14" s="50" t="n"/>
+      <c r="I14" s="50" t="n"/>
+      <c r="J14" s="11" t="n"/>
+      <c r="K14" s="13" t="n"/>
+      <c r="L14" s="13" t="n"/>
+      <c r="M14" s="14" t="n"/>
+      <c r="N14" s="11" t="n"/>
+      <c r="O14" s="13" t="n"/>
+      <c r="P14" s="13" t="n"/>
+      <c r="Q14" s="14" t="n"/>
+      <c r="R14" s="11" t="n"/>
+      <c r="S14" s="13" t="n"/>
+      <c r="T14" s="23" t="n"/>
+      <c r="U14" s="14" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="15" s="2">
       <c r="A15" s="42" t="inlineStr">
@@ -1068,14 +1028,14 @@
           <t>1:15-2:15</t>
         </is>
       </c>
-      <c r="B16" s="50" t="inlineStr">
+      <c r="B16" s="51" t="inlineStr">
         <is>
           <t>OS B305 teacher1</t>
         </is>
       </c>
-      <c r="C16" s="51" t="n"/>
-      <c r="D16" s="51" t="n"/>
-      <c r="E16" s="51" t="n"/>
+      <c r="C16" s="50" t="n"/>
+      <c r="D16" s="50" t="n"/>
+      <c r="E16" s="50" t="n"/>
       <c r="F16" s="48" t="inlineStr">
         <is>
           <t>AD B313 admin B1</t>
@@ -1096,42 +1056,18 @@
           <t>OS B317 teacher1 B4</t>
         </is>
       </c>
-      <c r="J16" s="50" t="inlineStr">
-        <is>
-          <t>OS B305 teacher1</t>
-        </is>
-      </c>
-      <c r="K16" s="51" t="n"/>
-      <c r="L16" s="51" t="n"/>
-      <c r="M16" s="51" t="n"/>
-      <c r="N16" s="48" t="inlineStr">
-        <is>
-          <t>WP-II B314 teacher4 B1</t>
-        </is>
-      </c>
-      <c r="O16" s="48" t="inlineStr">
-        <is>
-          <t>WP-II B313 teacher4 B2</t>
-        </is>
-      </c>
-      <c r="P16" s="48" t="inlineStr">
-        <is>
-          <t>WP-II B312 teacher4 B3</t>
-        </is>
-      </c>
-      <c r="Q16" s="52" t="inlineStr">
-        <is>
-          <t>WP-II B315 teacher4 B4</t>
-        </is>
-      </c>
-      <c r="R16" s="50" t="inlineStr">
-        <is>
-          <t>CG B305 teacher3</t>
-        </is>
-      </c>
-      <c r="S16" s="51" t="n"/>
-      <c r="T16" s="51" t="n"/>
-      <c r="U16" s="51" t="n"/>
+      <c r="J16" s="12" t="n"/>
+      <c r="K16" s="15" t="n"/>
+      <c r="L16" s="15" t="n"/>
+      <c r="M16" s="16" t="n"/>
+      <c r="N16" s="12" t="n"/>
+      <c r="O16" s="15" t="n"/>
+      <c r="P16" s="15" t="n"/>
+      <c r="Q16" s="24" t="n"/>
+      <c r="R16" s="12" t="n"/>
+      <c r="S16" s="15" t="n"/>
+      <c r="T16" s="15" t="n"/>
+      <c r="U16" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="17" s="2">
       <c r="A17" s="41" t="inlineStr">
@@ -1139,38 +1075,30 @@
           <t>2:15-3:15</t>
         </is>
       </c>
-      <c r="B17" s="50" t="inlineStr">
+      <c r="B17" s="51" t="inlineStr">
         <is>
           <t>AD B305 admin</t>
         </is>
       </c>
-      <c r="C17" s="51" t="n"/>
-      <c r="D17" s="51" t="n"/>
-      <c r="E17" s="51" t="n"/>
-      <c r="F17" s="51" t="n"/>
-      <c r="G17" s="51" t="n"/>
-      <c r="H17" s="51" t="n"/>
-      <c r="I17" s="51" t="n"/>
-      <c r="J17" s="50" t="inlineStr">
-        <is>
-          <t>AD B305 admin</t>
-        </is>
-      </c>
-      <c r="K17" s="51" t="n"/>
-      <c r="L17" s="51" t="n"/>
-      <c r="M17" s="51" t="n"/>
-      <c r="N17" s="51" t="n"/>
-      <c r="O17" s="51" t="n"/>
-      <c r="P17" s="51" t="n"/>
-      <c r="Q17" s="51" t="n"/>
-      <c r="R17" s="50" t="inlineStr">
-        <is>
-          <t>OOSE B305 teacher2</t>
-        </is>
-      </c>
-      <c r="S17" s="51" t="n"/>
-      <c r="T17" s="51" t="n"/>
-      <c r="U17" s="51" t="n"/>
+      <c r="C17" s="50" t="n"/>
+      <c r="D17" s="50" t="n"/>
+      <c r="E17" s="50" t="n"/>
+      <c r="F17" s="50" t="n"/>
+      <c r="G17" s="50" t="n"/>
+      <c r="H17" s="50" t="n"/>
+      <c r="I17" s="50" t="n"/>
+      <c r="J17" s="11" t="n"/>
+      <c r="K17" s="13" t="n"/>
+      <c r="L17" s="13" t="n"/>
+      <c r="M17" s="14" t="n"/>
+      <c r="N17" s="11" t="n"/>
+      <c r="O17" s="13" t="n"/>
+      <c r="P17" s="13" t="n"/>
+      <c r="Q17" s="25" t="n"/>
+      <c r="R17" s="11" t="n"/>
+      <c r="S17" s="13" t="n"/>
+      <c r="T17" s="13" t="n"/>
+      <c r="U17" s="14" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="18" s="2">
       <c r="A18" s="41" t="inlineStr">
@@ -1178,46 +1106,34 @@
           <t>3.15-4:15</t>
         </is>
       </c>
-      <c r="B18" s="50" t="inlineStr">
+      <c r="B18" s="51" t="inlineStr">
         <is>
           <t>ITC B305 teacher2</t>
         </is>
       </c>
-      <c r="C18" s="51" t="n"/>
-      <c r="D18" s="51" t="n"/>
-      <c r="E18" s="51" t="n"/>
-      <c r="F18" s="50" t="inlineStr">
+      <c r="C18" s="50" t="n"/>
+      <c r="D18" s="50" t="n"/>
+      <c r="E18" s="50" t="n"/>
+      <c r="F18" s="51" t="inlineStr">
         <is>
           <t>OS B305 teacher1</t>
         </is>
       </c>
-      <c r="G18" s="51" t="n"/>
-      <c r="H18" s="51" t="n"/>
-      <c r="I18" s="51" t="n"/>
-      <c r="J18" s="50" t="inlineStr">
-        <is>
-          <t>OOSE B305 teacher2</t>
-        </is>
-      </c>
-      <c r="K18" s="51" t="n"/>
-      <c r="L18" s="51" t="n"/>
-      <c r="M18" s="51" t="n"/>
-      <c r="N18" s="50" t="inlineStr">
-        <is>
-          <t>ITC B305 teacher2</t>
-        </is>
-      </c>
-      <c r="O18" s="51" t="n"/>
-      <c r="P18" s="51" t="n"/>
-      <c r="Q18" s="51" t="n"/>
-      <c r="R18" s="50" t="inlineStr">
-        <is>
-          <t>ITC B305 teacher2</t>
-        </is>
-      </c>
-      <c r="S18" s="51" t="n"/>
-      <c r="T18" s="51" t="n"/>
-      <c r="U18" s="51" t="n"/>
+      <c r="G18" s="50" t="n"/>
+      <c r="H18" s="50" t="n"/>
+      <c r="I18" s="50" t="n"/>
+      <c r="J18" s="12" t="n"/>
+      <c r="K18" s="15" t="n"/>
+      <c r="L18" s="15" t="n"/>
+      <c r="M18" s="16" t="n"/>
+      <c r="N18" s="12" t="n"/>
+      <c r="O18" s="15" t="n"/>
+      <c r="P18" s="15" t="n"/>
+      <c r="Q18" s="16" t="n"/>
+      <c r="R18" s="12" t="n"/>
+      <c r="S18" s="15" t="n"/>
+      <c r="T18" s="15" t="n"/>
+      <c r="U18" s="16" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="19" s="2">
       <c r="A19" s="41" t="inlineStr">
@@ -1229,26 +1145,22 @@
       <c r="C19" s="23" t="n"/>
       <c r="D19" s="23" t="n"/>
       <c r="E19" s="25" t="n"/>
-      <c r="F19" s="50" t="inlineStr">
+      <c r="F19" s="51" t="inlineStr">
         <is>
           <t>CG B305 teacher3</t>
         </is>
       </c>
-      <c r="G19" s="51" t="n"/>
-      <c r="H19" s="51" t="n"/>
-      <c r="I19" s="51" t="n"/>
+      <c r="G19" s="50" t="n"/>
+      <c r="H19" s="50" t="n"/>
+      <c r="I19" s="50" t="n"/>
       <c r="J19" s="17" t="n"/>
       <c r="K19" s="18" t="n"/>
       <c r="L19" s="18" t="n"/>
       <c r="M19" s="19" t="n"/>
-      <c r="N19" s="50" t="inlineStr">
-        <is>
-          <t>AD B305 admin</t>
-        </is>
-      </c>
-      <c r="O19" s="51" t="n"/>
-      <c r="P19" s="51" t="n"/>
-      <c r="Q19" s="51" t="n"/>
+      <c r="N19" s="11" t="n"/>
+      <c r="O19" s="13" t="n"/>
+      <c r="P19" s="13" t="n"/>
+      <c r="Q19" s="14" t="n"/>
       <c r="R19" s="11" t="n"/>
       <c r="S19" s="13" t="n"/>
       <c r="T19" s="13" t="n"/>
@@ -1337,7 +1249,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="33">
     <mergeCell ref="B15:U15"/>
     <mergeCell ref="A31:T31"/>
     <mergeCell ref="A7:U7"/>
@@ -1371,28 +1283,6 @@
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="R16:U16"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="R18:U18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="0" footer="0" header="0" left="0.2755905511811024" right="0.2755905511811024" top="0"/>

</xml_diff>

<commit_message>
Added custom EmailBackend for immediate email dispatch
</commit_message>
<xml_diff>
--- a/static/upload/temp_timetable.xlsx
+++ b/static/upload/temp_timetable.xlsx
@@ -421,10 +421,10 @@
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="12" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,7 +742,7 @@
     <row customHeight="1" ht="18" r="1" s="2">
       <c r="A1" s="43" t="inlineStr">
         <is>
-          <t>16/09/2019</t>
+          <t>27/10/2019</t>
         </is>
       </c>
       <c r="B1" s="31" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D13" s="48" t="inlineStr">
         <is>
-          <t>AD B313 admin B3</t>
+          <t>AD B310 admin B3</t>
         </is>
       </c>
       <c r="E13" s="48" t="inlineStr">
@@ -949,18 +949,54 @@
           <t>WP-II B316 teacher4 B4</t>
         </is>
       </c>
-      <c r="J13" s="12" t="n"/>
-      <c r="K13" s="15" t="n"/>
-      <c r="L13" s="15" t="n"/>
-      <c r="M13" s="16" t="n"/>
-      <c r="N13" s="12" t="n"/>
-      <c r="O13" s="15" t="n"/>
-      <c r="P13" s="15" t="n"/>
-      <c r="Q13" s="16" t="n"/>
-      <c r="R13" s="12" t="n"/>
-      <c r="S13" s="15" t="n"/>
-      <c r="T13" s="22" t="n"/>
-      <c r="U13" s="16" t="n"/>
+      <c r="J13" s="48" t="inlineStr">
+        <is>
+          <t>WP-II B314 teacher4 B1</t>
+        </is>
+      </c>
+      <c r="K13" s="48" t="inlineStr">
+        <is>
+          <t>OS B317 teacher1 B2</t>
+        </is>
+      </c>
+      <c r="L13" s="48" t="inlineStr">
+        <is>
+          <t>OOSE B315 teacher2 B3</t>
+        </is>
+      </c>
+      <c r="M13" s="48" t="inlineStr">
+        <is>
+          <t>AD B313 admin B4</t>
+        </is>
+      </c>
+      <c r="N13" s="50" t="inlineStr">
+        <is>
+          <t>CG B305 teacher3</t>
+        </is>
+      </c>
+      <c r="O13" s="51" t="n"/>
+      <c r="P13" s="51" t="n"/>
+      <c r="Q13" s="51" t="n"/>
+      <c r="R13" s="48" t="inlineStr">
+        <is>
+          <t>CG B310 teacher3 B1</t>
+        </is>
+      </c>
+      <c r="S13" s="48" t="inlineStr">
+        <is>
+          <t>WP-II B313 teacher4 B2</t>
+        </is>
+      </c>
+      <c r="T13" s="52" t="inlineStr">
+        <is>
+          <t>OS B317 teacher1 B3</t>
+        </is>
+      </c>
+      <c r="U13" s="48" t="inlineStr">
+        <is>
+          <t>OOSE B315 teacher2 B4</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="32.25" r="14" s="2">
       <c r="A14" s="42" t="inlineStr">
@@ -969,26 +1005,30 @@
 12:30</t>
         </is>
       </c>
-      <c r="B14" s="50" t="n"/>
-      <c r="C14" s="50" t="n"/>
-      <c r="D14" s="50" t="n"/>
-      <c r="E14" s="50" t="n"/>
-      <c r="F14" s="50" t="n"/>
-      <c r="G14" s="50" t="n"/>
-      <c r="H14" s="50" t="n"/>
-      <c r="I14" s="50" t="n"/>
-      <c r="J14" s="11" t="n"/>
-      <c r="K14" s="13" t="n"/>
-      <c r="L14" s="13" t="n"/>
-      <c r="M14" s="14" t="n"/>
-      <c r="N14" s="11" t="n"/>
-      <c r="O14" s="13" t="n"/>
-      <c r="P14" s="13" t="n"/>
-      <c r="Q14" s="14" t="n"/>
-      <c r="R14" s="11" t="n"/>
-      <c r="S14" s="13" t="n"/>
-      <c r="T14" s="23" t="n"/>
-      <c r="U14" s="14" t="n"/>
+      <c r="B14" s="51" t="n"/>
+      <c r="C14" s="51" t="n"/>
+      <c r="D14" s="51" t="n"/>
+      <c r="E14" s="51" t="n"/>
+      <c r="F14" s="51" t="n"/>
+      <c r="G14" s="51" t="n"/>
+      <c r="H14" s="51" t="n"/>
+      <c r="I14" s="51" t="n"/>
+      <c r="J14" s="51" t="n"/>
+      <c r="K14" s="51" t="n"/>
+      <c r="L14" s="51" t="n"/>
+      <c r="M14" s="51" t="n"/>
+      <c r="N14" s="50" t="inlineStr">
+        <is>
+          <t>OOSE B305 teacher2</t>
+        </is>
+      </c>
+      <c r="O14" s="51" t="n"/>
+      <c r="P14" s="51" t="n"/>
+      <c r="Q14" s="51" t="n"/>
+      <c r="R14" s="51" t="n"/>
+      <c r="S14" s="51" t="n"/>
+      <c r="T14" s="51" t="n"/>
+      <c r="U14" s="51" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="15" s="2">
       <c r="A15" s="42" t="inlineStr">
@@ -1028,14 +1068,14 @@
           <t>1:15-2:15</t>
         </is>
       </c>
-      <c r="B16" s="51" t="inlineStr">
+      <c r="B16" s="50" t="inlineStr">
         <is>
           <t>OS B305 teacher1</t>
         </is>
       </c>
-      <c r="C16" s="50" t="n"/>
-      <c r="D16" s="50" t="n"/>
-      <c r="E16" s="50" t="n"/>
+      <c r="C16" s="51" t="n"/>
+      <c r="D16" s="51" t="n"/>
+      <c r="E16" s="51" t="n"/>
       <c r="F16" s="48" t="inlineStr">
         <is>
           <t>AD B313 admin B1</t>
@@ -1056,18 +1096,42 @@
           <t>OS B317 teacher1 B4</t>
         </is>
       </c>
-      <c r="J16" s="12" t="n"/>
-      <c r="K16" s="15" t="n"/>
-      <c r="L16" s="15" t="n"/>
-      <c r="M16" s="16" t="n"/>
-      <c r="N16" s="12" t="n"/>
-      <c r="O16" s="15" t="n"/>
-      <c r="P16" s="15" t="n"/>
-      <c r="Q16" s="24" t="n"/>
-      <c r="R16" s="12" t="n"/>
-      <c r="S16" s="15" t="n"/>
-      <c r="T16" s="15" t="n"/>
-      <c r="U16" s="16" t="n"/>
+      <c r="J16" s="50" t="inlineStr">
+        <is>
+          <t>OS B305 teacher1</t>
+        </is>
+      </c>
+      <c r="K16" s="51" t="n"/>
+      <c r="L16" s="51" t="n"/>
+      <c r="M16" s="51" t="n"/>
+      <c r="N16" s="48" t="inlineStr">
+        <is>
+          <t>WP-II B314 teacher4 B1</t>
+        </is>
+      </c>
+      <c r="O16" s="48" t="inlineStr">
+        <is>
+          <t>WP-II B313 teacher4 B2</t>
+        </is>
+      </c>
+      <c r="P16" s="48" t="inlineStr">
+        <is>
+          <t>WP-II B312 teacher4 B3</t>
+        </is>
+      </c>
+      <c r="Q16" s="52" t="inlineStr">
+        <is>
+          <t>WP-II B315 teacher4 B4</t>
+        </is>
+      </c>
+      <c r="R16" s="50" t="inlineStr">
+        <is>
+          <t>CG B305 teacher3</t>
+        </is>
+      </c>
+      <c r="S16" s="51" t="n"/>
+      <c r="T16" s="51" t="n"/>
+      <c r="U16" s="51" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="17" s="2">
       <c r="A17" s="41" t="inlineStr">
@@ -1075,30 +1139,38 @@
           <t>2:15-3:15</t>
         </is>
       </c>
-      <c r="B17" s="51" t="inlineStr">
+      <c r="B17" s="50" t="inlineStr">
         <is>
           <t>AD B305 admin</t>
         </is>
       </c>
-      <c r="C17" s="50" t="n"/>
-      <c r="D17" s="50" t="n"/>
-      <c r="E17" s="50" t="n"/>
-      <c r="F17" s="50" t="n"/>
-      <c r="G17" s="50" t="n"/>
-      <c r="H17" s="50" t="n"/>
-      <c r="I17" s="50" t="n"/>
-      <c r="J17" s="11" t="n"/>
-      <c r="K17" s="13" t="n"/>
-      <c r="L17" s="13" t="n"/>
-      <c r="M17" s="14" t="n"/>
-      <c r="N17" s="11" t="n"/>
-      <c r="O17" s="13" t="n"/>
-      <c r="P17" s="13" t="n"/>
-      <c r="Q17" s="25" t="n"/>
-      <c r="R17" s="11" t="n"/>
-      <c r="S17" s="13" t="n"/>
-      <c r="T17" s="13" t="n"/>
-      <c r="U17" s="14" t="n"/>
+      <c r="C17" s="51" t="n"/>
+      <c r="D17" s="51" t="n"/>
+      <c r="E17" s="51" t="n"/>
+      <c r="F17" s="51" t="n"/>
+      <c r="G17" s="51" t="n"/>
+      <c r="H17" s="51" t="n"/>
+      <c r="I17" s="51" t="n"/>
+      <c r="J17" s="50" t="inlineStr">
+        <is>
+          <t>AD B305 admin</t>
+        </is>
+      </c>
+      <c r="K17" s="51" t="n"/>
+      <c r="L17" s="51" t="n"/>
+      <c r="M17" s="51" t="n"/>
+      <c r="N17" s="51" t="n"/>
+      <c r="O17" s="51" t="n"/>
+      <c r="P17" s="51" t="n"/>
+      <c r="Q17" s="51" t="n"/>
+      <c r="R17" s="50" t="inlineStr">
+        <is>
+          <t>OOSE B305 teacher2</t>
+        </is>
+      </c>
+      <c r="S17" s="51" t="n"/>
+      <c r="T17" s="51" t="n"/>
+      <c r="U17" s="51" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="18" s="2">
       <c r="A18" s="41" t="inlineStr">
@@ -1106,34 +1178,46 @@
           <t>3.15-4:15</t>
         </is>
       </c>
-      <c r="B18" s="51" t="inlineStr">
+      <c r="B18" s="50" t="inlineStr">
         <is>
           <t>ITC B305 teacher2</t>
         </is>
       </c>
-      <c r="C18" s="50" t="n"/>
-      <c r="D18" s="50" t="n"/>
-      <c r="E18" s="50" t="n"/>
-      <c r="F18" s="51" t="inlineStr">
+      <c r="C18" s="51" t="n"/>
+      <c r="D18" s="51" t="n"/>
+      <c r="E18" s="51" t="n"/>
+      <c r="F18" s="50" t="inlineStr">
         <is>
           <t>OS B305 teacher1</t>
         </is>
       </c>
-      <c r="G18" s="50" t="n"/>
-      <c r="H18" s="50" t="n"/>
-      <c r="I18" s="50" t="n"/>
-      <c r="J18" s="12" t="n"/>
-      <c r="K18" s="15" t="n"/>
-      <c r="L18" s="15" t="n"/>
-      <c r="M18" s="16" t="n"/>
-      <c r="N18" s="12" t="n"/>
-      <c r="O18" s="15" t="n"/>
-      <c r="P18" s="15" t="n"/>
-      <c r="Q18" s="16" t="n"/>
-      <c r="R18" s="12" t="n"/>
-      <c r="S18" s="15" t="n"/>
-      <c r="T18" s="15" t="n"/>
-      <c r="U18" s="16" t="n"/>
+      <c r="G18" s="51" t="n"/>
+      <c r="H18" s="51" t="n"/>
+      <c r="I18" s="51" t="n"/>
+      <c r="J18" s="50" t="inlineStr">
+        <is>
+          <t>OOSE B305 teacher2</t>
+        </is>
+      </c>
+      <c r="K18" s="51" t="n"/>
+      <c r="L18" s="51" t="n"/>
+      <c r="M18" s="51" t="n"/>
+      <c r="N18" s="50" t="inlineStr">
+        <is>
+          <t>ITC B305 teacher2</t>
+        </is>
+      </c>
+      <c r="O18" s="51" t="n"/>
+      <c r="P18" s="51" t="n"/>
+      <c r="Q18" s="51" t="n"/>
+      <c r="R18" s="50" t="inlineStr">
+        <is>
+          <t>ITC B305 teacher2</t>
+        </is>
+      </c>
+      <c r="S18" s="51" t="n"/>
+      <c r="T18" s="51" t="n"/>
+      <c r="U18" s="51" t="n"/>
     </row>
     <row customHeight="1" ht="32.25" r="19" s="2">
       <c r="A19" s="41" t="inlineStr">
@@ -1145,22 +1229,26 @@
       <c r="C19" s="23" t="n"/>
       <c r="D19" s="23" t="n"/>
       <c r="E19" s="25" t="n"/>
-      <c r="F19" s="51" t="inlineStr">
+      <c r="F19" s="50" t="inlineStr">
         <is>
           <t>CG B305 teacher3</t>
         </is>
       </c>
-      <c r="G19" s="50" t="n"/>
-      <c r="H19" s="50" t="n"/>
-      <c r="I19" s="50" t="n"/>
+      <c r="G19" s="51" t="n"/>
+      <c r="H19" s="51" t="n"/>
+      <c r="I19" s="51" t="n"/>
       <c r="J19" s="17" t="n"/>
       <c r="K19" s="18" t="n"/>
       <c r="L19" s="18" t="n"/>
       <c r="M19" s="19" t="n"/>
-      <c r="N19" s="11" t="n"/>
-      <c r="O19" s="13" t="n"/>
-      <c r="P19" s="13" t="n"/>
-      <c r="Q19" s="14" t="n"/>
+      <c r="N19" s="50" t="inlineStr">
+        <is>
+          <t>AD B305 admin</t>
+        </is>
+      </c>
+      <c r="O19" s="51" t="n"/>
+      <c r="P19" s="51" t="n"/>
+      <c r="Q19" s="51" t="n"/>
       <c r="R19" s="11" t="n"/>
       <c r="S19" s="13" t="n"/>
       <c r="T19" s="13" t="n"/>
@@ -1249,7 +1337,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="55">
     <mergeCell ref="B15:U15"/>
     <mergeCell ref="A31:T31"/>
     <mergeCell ref="A7:U7"/>
@@ -1283,6 +1371,28 @@
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="R16:U16"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="R18:U18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins bottom="0" footer="0" header="0" left="0.2755905511811024" right="0.2755905511811024" top="0"/>

</xml_diff>